<commit_message>
AJUSTES NA PLANILHA DE CONTROLE
</commit_message>
<xml_diff>
--- a/Controle/Controle das Atividades.xlsx
+++ b/Controle/Controle das Atividades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Victor</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo </t>
-  </si>
-  <si>
     <t>Ativo</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Reunião 25/09</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>GERAL</t>
   </si>
   <si>
@@ -88,6 +82,24 @@
   </si>
   <si>
     <t>Ativo2</t>
+  </si>
+  <si>
+    <t>Ativo3</t>
+  </si>
+  <si>
+    <t>Concordou2</t>
+  </si>
+  <si>
+    <t>Compareceu2</t>
+  </si>
+  <si>
+    <t>Grupo2</t>
+  </si>
+  <si>
+    <t>Grupo3</t>
+  </si>
+  <si>
+    <t>Reunião 24/09</t>
   </si>
 </sst>
 </file>
@@ -103,12 +115,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,16 +147,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -146,19 +244,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B4:I15" totalsRowShown="0">
-  <autoFilter ref="B4:I15"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B4:M15" totalsRowShown="0">
+  <autoFilter ref="B4:M15"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Membros"/>
     <tableColumn id="2" name="Email"/>
     <tableColumn id="9" name="Grupo"/>
     <tableColumn id="8" name="Ativo"/>
-    <tableColumn id="3" name="Grupo "/>
-    <tableColumn id="4" name="Ativo2"/>
-    <tableColumn id="7" name="Concordou"/>
-    <tableColumn id="5" name="Compareceu"/>
+    <tableColumn id="3" name="Grupo2" dataDxfId="4"/>
+    <tableColumn id="6" name="Ativo2" dataDxfId="3"/>
+    <tableColumn id="10" name="Concordou" dataDxfId="2"/>
+    <tableColumn id="11" name="Compareceu" dataDxfId="1"/>
+    <tableColumn id="12" name="Grupo3" dataDxfId="0"/>
+    <tableColumn id="4" name="Ativo3" dataDxfId="7"/>
+    <tableColumn id="7" name="Concordou2" dataDxfId="6"/>
+    <tableColumn id="5" name="Compareceu2" dataDxfId="5"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -425,261 +527,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I15"/>
+  <dimension ref="B3:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="6" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="N3:Q3"/>
     <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="J3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
ATUALIZAÇÕES NO CONTROLE DAS ATIVIDADES
</commit_message>
<xml_diff>
--- a/Controle/Controle das Atividades.xlsx
+++ b/Controle/Controle das Atividades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
   <si>
     <t>Victor</t>
   </si>
@@ -149,18 +149,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,14 +251,14 @@
     <tableColumn id="2" name="Email"/>
     <tableColumn id="9" name="Grupo"/>
     <tableColumn id="8" name="Ativo"/>
-    <tableColumn id="3" name="Grupo2" dataDxfId="4"/>
-    <tableColumn id="6" name="Ativo2" dataDxfId="3"/>
-    <tableColumn id="10" name="Concordou" dataDxfId="2"/>
-    <tableColumn id="11" name="Compareceu" dataDxfId="1"/>
-    <tableColumn id="12" name="Grupo3" dataDxfId="0"/>
-    <tableColumn id="4" name="Ativo3" dataDxfId="7"/>
-    <tableColumn id="7" name="Concordou2" dataDxfId="6"/>
-    <tableColumn id="5" name="Compareceu2" dataDxfId="5"/>
+    <tableColumn id="3" name="Grupo2" dataDxfId="7"/>
+    <tableColumn id="6" name="Ativo2" dataDxfId="6"/>
+    <tableColumn id="10" name="Concordou" dataDxfId="5"/>
+    <tableColumn id="11" name="Compareceu" dataDxfId="4"/>
+    <tableColumn id="12" name="Grupo3" dataDxfId="3"/>
+    <tableColumn id="4" name="Ativo3" dataDxfId="2"/>
+    <tableColumn id="7" name="Concordou2" dataDxfId="1"/>
+    <tableColumn id="5" name="Compareceu2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,7 +530,7 @@
   <dimension ref="B3:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,64 +544,64 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="2" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -612,18 +612,18 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -632,14 +632,16 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -648,14 +650,22 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -664,18 +674,20 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -687,24 +699,26 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -716,22 +730,24 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -743,26 +759,28 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="4"/>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -774,24 +792,24 @@
       <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="4"/>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -800,18 +818,18 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -820,14 +838,20 @@
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -839,24 +863,24 @@
       <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="4"/>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>